<commit_message>
Update dữ liệu khai báo mới ngày 30/05/2025
</commit_message>
<xml_diff>
--- a/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
+++ b/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E604FEDE-75F8-4266-B524-E8E495D0D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E86CEC-9B06-4A8D-BD20-C4F6A044846E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB3A4D1C-0848-4C13-8670-93B20E72328E}"/>
   </bookViews>
@@ -567,7 +567,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -648,12 +648,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,6 +706,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1013,10 +1027,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,6 +2353,11 @@
         <v>Ảnh mặt sau</v>
       </c>
     </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cập nhật dữ liệu khai báo lưu trú ngày 30/05/2025
</commit_message>
<xml_diff>
--- a/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
+++ b/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA54F05B-628F-4DF0-886D-5DD5A7C422B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDA5865-984C-401C-91ED-49536C2E8431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB3A4D1C-0848-4C13-8670-93B20E72328E}"/>
   </bookViews>
@@ -567,7 +567,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -648,23 +648,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -706,9 +695,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1027,10 +1013,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,12 +2339,6 @@
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
-        <v>1</v>
-      </c>
-      <c r="B35" s="15"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sao lưu dữ liệu khai báo lưu trú 31/05/2025
</commit_message>
<xml_diff>
--- a/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
+++ b/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDA5865-984C-401C-91ED-49536C2E8431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E84DB30-2C59-4060-95F5-778E46D76AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB3A4D1C-0848-4C13-8670-93B20E72328E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="169">
   <si>
     <t>Số giấy tờ</t>
   </si>
@@ -510,6 +510,42 @@
   </si>
   <si>
     <t>22:33:10 29/05/2025</t>
+  </si>
+  <si>
+    <t>Nguyễn Đức Định</t>
+  </si>
+  <si>
+    <t>Thôn Đông Bình, Nhơn Thọ, Thị xã An Nhơn, Bình Định</t>
+  </si>
+  <si>
+    <t>20/01/2023</t>
+  </si>
+  <si>
+    <t>20:46:22 30/05/2025</t>
+  </si>
+  <si>
+    <t>Nguyễn Lâm Mỹ Phượng</t>
+  </si>
+  <si>
+    <t>Khu Vực 2, Trà Lồng, TX. Long Mỹ, Hậu Giang</t>
+  </si>
+  <si>
+    <t>16/12/2024</t>
+  </si>
+  <si>
+    <t>21:04:39 31/05/2025</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Hải</t>
+  </si>
+  <si>
+    <t>28/02/1999</t>
+  </si>
+  <si>
+    <t>Khóm Trung 3, Thị trấn Phú Mỹ, Phú Tân, An Giang</t>
+  </si>
+  <si>
+    <t>21:07:11 31/05/2025</t>
   </si>
 </sst>
 </file>
@@ -567,7 +603,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -601,19 +637,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -629,22 +652,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -653,15 +661,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -670,31 +672,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1013,7 +1003,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD35"/>
@@ -1036,1306 +1026,1422 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>91095006338</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>371727089</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="7" t="str">
+      <c r="K2" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_Le_Quoc_Hiep_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L2" s="7" t="str">
+      <c r="L2" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_sau_Le_Quoc_Hiep_19_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>96193007157</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>33970</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="2" t="str">
+      <c r="K3" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_NGUYEN_THI_BICH_VAN_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L3" s="2" t="str">
+      <c r="L3" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_sau_NGUYEN_THI_BICH_VAN_19_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>56194006799</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="2" t="str">
+      <c r="K4" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_TRAN_TIN_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>82079009889</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>25726188</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="2" t="str">
+      <c r="K5" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Huy_Binh_20_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L5" s="2" t="str">
+      <c r="L5" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Huy_Binh_20_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>75202005210</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="2" t="str">
+      <c r="K6" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_PHAN_HOANG_HIEU_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>51084019055</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>212772204</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4">
         <v>30682</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="2" t="str">
+      <c r="K7" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Duc_Danh_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L7" s="2" t="str">
+      <c r="L7" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Duc_Danh_21_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>91301013069</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>372037622</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="2" t="str">
+      <c r="K8" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Phuong_Thanh_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>89206019981</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4">
         <v>38751</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="2" t="str">
+      <c r="K9" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_PHAM_THANH_DONG_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>79095002950</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>25463058</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="2" t="str">
+      <c r="K10" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Tran_Phuc_Hau_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L10" s="2" t="str">
+      <c r="L10" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Tran_Phuc_Hau_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>91078008986</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>352465981</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="2" t="str">
+      <c r="K11" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Ngoc_Hong_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L11" s="2" t="str">
+      <c r="L11" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Ngoc_Hong_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>91097015554</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>371901334</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4">
         <v>35709</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="2" t="str">
+      <c r="K12" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_The_Hai_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L12" s="2" t="str">
+      <c r="L12" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_The_Hai_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>91071015623</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>371307162</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="2" t="str">
+      <c r="K13" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Thanh_Tuan_23_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L13" s="2" t="str">
+      <c r="L13" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Thanh_Tuan_23_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>87096015542</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K14" s="2" t="str">
+      <c r="K14" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_NGUYEN_MINH_TIEN_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L14" s="2" t="str">
+      <c r="L14" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_NGUYEN_MINH_TIEN_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>91081017072</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>370841245</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4">
         <v>29587</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K15" s="2" t="str">
+      <c r="K15" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L15" s="2" t="str">
+      <c r="L15" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>91084012750</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>370990818</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4">
         <v>30750</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K16" s="2" t="str">
+      <c r="K16" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Thanh_Viet_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L16" s="2" t="str">
+      <c r="L16" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Thanh_Viet_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>1080001692</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>11897042</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="4">
         <v>45111</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K17" s="2" t="str">
+      <c r="K17" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Bui_Xuan_Khang_25_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L17" s="1"/>
+      <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="2">
         <v>93089002224</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="2">
         <v>363625191</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="13" t="s">
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="K18" s="14" t="str">
+      <c r="K18" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231015986_1f8b3e3bff5db9556942e37df55eced1.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L18" s="14" t="str">
+      <c r="L18" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231009013_d0555d63762caa707a528779cd4b389d.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="2">
         <v>92202000529</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="11">
+      <c r="D19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="4">
         <v>37349</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="4">
         <v>44412</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K19" s="7" t="str">
+      <c r="K19" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638567942044_da6c7396bdb2fd41771af011ea2145c5.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L19" s="7" t="str">
+      <c r="L19" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638568010435_4cb996aca8b62ce8c532ac2c778dde52.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="2">
         <v>91086020674</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="2">
         <v>371101463</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="9">
+      <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="4">
         <v>31417</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="8" t="s">
+      <c r="H20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K20" s="10" t="str">
+      <c r="K20" s="5" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Phan_Ngoc_Dang_26_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L20" s="10" t="str">
+      <c r="L20" s="5" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Phan_Ngoc_Dang_26_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="2">
         <v>1073013937</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="2">
         <v>23081798</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="6" t="s">
+      <c r="H21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K21" s="7" t="str">
+      <c r="K21" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641706780560_8de2b94abdddf01864418a9ee361f149.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L21" s="7" t="str">
+      <c r="L21" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641706753500_4969ef17448d95fa7b72914b4214e313.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>89191014033</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>352357017</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="H22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K22" s="2" t="str">
+      <c r="K22" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641780724942_fb1294927028398d7950862fa21f9636.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L22" s="2" t="str">
+      <c r="L22" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641780715963_324045fc09999ad0544e5e88e11e507e.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>89195008544</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="H23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K23" s="2" t="str">
+      <c r="K23" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641990529491_dc032a7b7fed2b70e37151d2a537d76a.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L23" s="2" t="str">
+      <c r="L23" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641990535137_0ba3595f83c73ecf5e97519d7e4f843a.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>91308000131</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="H24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K24" s="2" t="str">
+      <c r="K24" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6644316579444_f67de388d3d57ed3ae9a5e8306dccebb.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L24" s="2" t="str">
+      <c r="L24" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6644316567657_6d508f7fbad3b912ebad7c3a2bde4ede.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>91090022191</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="1" t="s">
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="K25" s="2" t="str">
+      <c r="K25" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645679784460_16e9831700eec884b4672019a8e5bfd8.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L25" s="2" t="str">
+      <c r="L25" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645679849486_f2d97fe44df1a882fee4c3e556b460d2.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>87205017175</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>372056275</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="4">
         <v>45452</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="1" t="s">
+      <c r="H26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="2" t="str">
+      <c r="K26" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718598837_bba874eeeaee72f671be148520fa04b0.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L26" s="2" t="str">
+      <c r="L26" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718650512_7337cb5b825ec0567cc8354ba1923a63.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>86093011875</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>331682224</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="D27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="4">
         <v>44477</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="H27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K27" s="2" t="str">
+      <c r="K27" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718626247_43b23736a79c792015edd2e82b865f50.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L27" s="2" t="str">
+      <c r="L27" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718611344_84cf2a06806039ffa53b154dec78a339.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>91301013069</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>372037622</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="H28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K28" s="2" t="str">
+      <c r="K28" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6648835576244_a2b952b7970c5b96f3efe8aec6c5c6fe.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L28" s="1"/>
+      <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>91086004502</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="D29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="4">
         <v>31503</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="4">
         <v>45055</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="1" t="s">
+      <c r="H29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="K29" s="2" t="str">
+      <c r="K29" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6649363260209_12712fa4552842f9089d02cedb55b602.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L29" s="2" t="str">
+      <c r="L29" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6649363228340_9751bb18278ccc22aacbd35eeb4c3ab9.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>38203017024</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="1" t="s">
+      <c r="H30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="K30" s="2" t="str">
+      <c r="K30" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078531533_66d3cde5f7ba221f3215adeb3f6e8484.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L30" s="2" t="str">
+      <c r="L30" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078408443_5b3a0f504d4db5db6ac51ae06d0115b1.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>79089035969</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>24228060</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="D31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="H31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J31" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K31" s="2" t="str">
+      <c r="K31" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6652066448631_e17daed702f5eb47520dac0a1edf6c01.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L31" s="2" t="str">
+      <c r="L31" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6652066391227_9ea3764b58b18c3479c831a588aef359.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <v>38203017024</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="4" t="s">
+      <c r="H32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K32" s="5" t="str">
+      <c r="K32" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078531533_66d3cde5f7ba221f3215adeb3f6e8484.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L32" s="5" t="str">
+      <c r="L32" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078408443_5b3a0f504d4db5db6ac51ae06d0115b1.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="2">
         <v>91086020674</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="2">
         <v>371101463</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="9">
+      <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="4">
         <v>31417</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="8" t="s">
+      <c r="H33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
+      <c r="A34" s="2">
         <v>93089002224</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="2">
         <v>363625191</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="13" t="s">
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="13" t="s">
+      <c r="H34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K34" s="14" t="str">
+      <c r="K34" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231015986_1f8b3e3bff5db9556942e37df55eced1.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L34" s="14" t="str">
+      <c r="L34" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231009013_d0555d63762caa707a528779cd4b389d.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>52095016049</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="4">
+        <v>34792</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K35" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6655770392067_dac28a538906af34430c537091b09146.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L35" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6655770441419_e8c4a4d84d72e6900b06838210a76a8b.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>93300005349</v>
+      </c>
+      <c r="B36" s="2">
+        <v>364095686</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="4">
+        <v>36526</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K36" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658662217643_ed95c6620651e7d00cbf14056e8b76fb.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L36" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658662210545_e4ce0c32a1d467887e7833d12cb4a286.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>89099008678</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="7">
+        <v>44688</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="K37" s="8" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658663234407_49b889c545ea800460ccfc5bd004abfc.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L37" s="8" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658663793134_2c4e81af8d38d8105d9c2186365b1a58.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sao lưu dữ liệu ngày 31/05/2025
</commit_message>
<xml_diff>
--- a/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
+++ b/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E84DB30-2C59-4060-95F5-778E46D76AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15909A5-4D21-4CCF-B7A4-C53C4AEE2DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB3A4D1C-0848-4C13-8670-93B20E72328E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$J$1:$J$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="180">
   <si>
     <t>Số giấy tờ</t>
   </si>
@@ -546,6 +546,39 @@
   </si>
   <si>
     <t>21:07:11 31/05/2025</t>
+  </si>
+  <si>
+    <t>Trần Nhựt Bổn</t>
+  </si>
+  <si>
+    <t>16/01/1988</t>
+  </si>
+  <si>
+    <t>Tổ 6, Ấp Hậu Giang 2, Tân Hòa, Phú Tân, An Giang</t>
+  </si>
+  <si>
+    <t>14/06/2023</t>
+  </si>
+  <si>
+    <t>21:38:14 31/05/2025</t>
+  </si>
+  <si>
+    <t>21:54:40 31/05/2025</t>
+  </si>
+  <si>
+    <t>Ngô Xuân Trọng</t>
+  </si>
+  <si>
+    <t>28/08/2005</t>
+  </si>
+  <si>
+    <t>Ấp Phụng Thạnh, Thạnh Tiến, Vĩnh Thạnh, Cần Thơ</t>
+  </si>
+  <si>
+    <t>13/05/2021</t>
+  </si>
+  <si>
+    <t>21:55:02 31/05/2025</t>
   </si>
 </sst>
 </file>
@@ -603,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -637,6 +670,19 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -652,7 +698,22 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,9 +722,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -672,19 +742,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1002,11 +1084,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L37"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,1426 +1108,1553 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>91095006338</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="7">
         <v>371727089</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="3" t="str">
+      <c r="K2" s="8" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_Le_Quoc_Hiep_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L2" s="3" t="str">
+      <c r="L2" s="8" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_sau_Le_Quoc_Hiep_19_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>96193007157</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>33970</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="3" t="str">
+      <c r="K3" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_NGUYEN_THI_BICH_VAN_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L3" s="3" t="str">
+      <c r="L3" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_sau_NGUYEN_THI_BICH_VAN_19_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>56194006799</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="3" t="str">
+      <c r="K4" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_TRAN_TIN_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>82079009889</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>25726188</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="3" t="str">
+      <c r="K5" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Huy_Binh_20_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L5" s="3" t="str">
+      <c r="L5" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Huy_Binh_20_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>75202005210</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="3" t="str">
+      <c r="K6" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_PHAN_HOANG_HIEU_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>51084019055</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>212772204</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
         <v>30682</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="3" t="str">
+      <c r="K7" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Duc_Danh_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L7" s="3" t="str">
+      <c r="L7" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Duc_Danh_21_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>91301013069</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>372037622</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="3" t="str">
+      <c r="K8" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Phuong_Thanh_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>89206019981</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3">
         <v>38751</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="2" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="3" t="str">
+      <c r="K9" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_PHAM_THANH_DONG_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>79095002950</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>25463058</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="3" t="str">
+      <c r="K10" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Tran_Phuc_Hau_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L10" s="3" t="str">
+      <c r="L10" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Tran_Phuc_Hau_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>91078008986</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>352465981</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="3" t="str">
+      <c r="K11" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Ngoc_Hong_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L11" s="3" t="str">
+      <c r="L11" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Ngoc_Hong_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>91097015554</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>371901334</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3">
         <v>35709</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2" t="s">
+      <c r="H12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="3" t="str">
+      <c r="K12" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_The_Hai_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L12" s="3" t="str">
+      <c r="L12" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_The_Hai_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>91071015623</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>371307162</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="3" t="str">
+      <c r="K13" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Thanh_Tuan_23_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L13" s="3" t="str">
+      <c r="L13" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Thanh_Tuan_23_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>87096015542</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="H14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K14" s="3" t="str">
+      <c r="K14" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_NGUYEN_MINH_TIEN_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L14" s="3" t="str">
+      <c r="L14" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_NGUYEN_MINH_TIEN_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="11">
         <v>91081017072</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="11">
         <v>370841245</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="12">
         <v>29587</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="2" t="s">
+      <c r="H15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="K15" s="3" t="str">
+      <c r="K15" s="13" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L15" s="3" t="str">
+      <c r="L15" s="13" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>91084012750</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="7">
         <v>370990818</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="D16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="9">
         <v>30750</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="2" t="s">
+      <c r="H16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K16" s="3" t="str">
+      <c r="K16" s="8" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Thanh_Viet_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L16" s="3" t="str">
+      <c r="L16" s="8" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Thanh_Viet_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>1080001692</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>11897042</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>45111</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K17" s="3" t="str">
+      <c r="K17" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Bui_Xuan_Khang_25_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>93089002224</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>363625191</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K18" s="3" t="str">
+      <c r="K18" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231015986_1f8b3e3bff5db9556942e37df55eced1.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L18" s="3" t="str">
+      <c r="L18" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231009013_d0555d63762caa707a528779cd4b389d.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>92202000529</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="4">
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="3">
         <v>37349</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>44412</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="2" t="s">
+      <c r="H19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K19" s="3" t="str">
+      <c r="K19" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638567942044_da6c7396bdb2fd41771af011ea2145c5.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L19" s="3" t="str">
+      <c r="L19" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638568010435_4cb996aca8b62ce8c532ac2c778dde52.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>91086020674</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>371101463</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="3">
         <v>31417</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="2" t="s">
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K20" s="5" t="str">
+      <c r="K20" s="4" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Phan_Ngoc_Dang_26_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L20" s="5" t="str">
+      <c r="L20" s="4" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Phan_Ngoc_Dang_26_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>1073013937</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>23081798</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="H21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K21" s="3" t="str">
+      <c r="K21" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641706780560_8de2b94abdddf01864418a9ee361f149.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L21" s="3" t="str">
+      <c r="L21" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641706753500_4969ef17448d95fa7b72914b4214e313.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>89191014033</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>352357017</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K22" s="3" t="str">
+      <c r="K22" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641780724942_fb1294927028398d7950862fa21f9636.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L22" s="3" t="str">
+      <c r="L22" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641780715963_324045fc09999ad0544e5e88e11e507e.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>89195008544</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="H23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="K23" s="3" t="str">
+      <c r="K23" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641990529491_dc032a7b7fed2b70e37151d2a537d76a.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L23" s="3" t="str">
+      <c r="L23" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641990535137_0ba3595f83c73ecf5e97519d7e4f843a.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>91308000131</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="2" t="s">
+      <c r="H24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K24" s="3" t="str">
+      <c r="K24" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6644316579444_f67de388d3d57ed3ae9a5e8306dccebb.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L24" s="3" t="str">
+      <c r="L24" s="2" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6644316567657_6d508f7fbad3b912ebad7c3a2bde4ede.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>91090022191</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="H25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="K25" s="3" t="str">
+      <c r="K25" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645679784460_16e9831700eec884b4672019a8e5bfd8.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L25" s="3" t="str">
+      <c r="L25" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645679849486_f2d97fe44df1a882fee4c3e556b460d2.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>87205017175</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>372056275</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>45452</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="2" t="s">
+      <c r="H26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="3" t="str">
+      <c r="K26" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718598837_bba874eeeaee72f671be148520fa04b0.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L26" s="3" t="str">
+      <c r="L26" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718650512_7337cb5b825ec0567cc8354ba1923a63.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>86093011875</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>331682224</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>44477</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="2" t="s">
+      <c r="H27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K27" s="3" t="str">
+      <c r="K27" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718626247_43b23736a79c792015edd2e82b865f50.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L27" s="3" t="str">
+      <c r="L27" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718611344_84cf2a06806039ffa53b154dec78a339.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>91301013069</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>372037622</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="H28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K28" s="3" t="str">
+      <c r="K28" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6648835576244_a2b952b7970c5b96f3efe8aec6c5c6fe.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>91086004502</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="4">
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="3">
         <v>31503</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>45055</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="2" t="s">
+      <c r="H29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K29" s="3" t="str">
+      <c r="K29" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6649363260209_12712fa4552842f9089d02cedb55b602.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L29" s="3" t="str">
+      <c r="L29" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6649363228340_9751bb18278ccc22aacbd35eeb4c3ab9.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>38203017024</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="D30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="2" t="s">
+      <c r="H30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K30" s="3" t="str">
+      <c r="K30" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078531533_66d3cde5f7ba221f3215adeb3f6e8484.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L30" s="3" t="str">
+      <c r="L30" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078408443_5b3a0f504d4db5db6ac51ae06d0115b1.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>79089035969</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>24228060</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="2" t="s">
+      <c r="H31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K31" s="3" t="str">
+      <c r="K31" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6652066448631_e17daed702f5eb47520dac0a1edf6c01.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L31" s="3" t="str">
+      <c r="L31" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6652066391227_9ea3764b58b18c3479c831a588aef359.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>38203017024</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="2" t="s">
+      <c r="H32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K32" s="3" t="str">
+      <c r="K32" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078531533_66d3cde5f7ba221f3215adeb3f6e8484.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L32" s="3" t="str">
+      <c r="L32" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078408443_5b3a0f504d4db5db6ac51ae06d0115b1.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>91086020674</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>371101463</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="4">
+      <c r="D33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="3">
         <v>31417</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="H33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>93089002224</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>363625191</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="D34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="2" t="s">
+      <c r="H34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K34" s="3" t="str">
+      <c r="K34" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231015986_1f8b3e3bff5db9556942e37df55eced1.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L34" s="3" t="str">
+      <c r="L34" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231009013_d0555d63762caa707a528779cd4b389d.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>52095016049</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="4">
+      <c r="D35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="3">
         <v>34792</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="2" t="s">
+      <c r="H35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="K35" s="3" t="str">
+      <c r="K35" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6655770392067_dac28a538906af34430c537091b09146.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L35" s="3" t="str">
+      <c r="L35" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6655770441419_e8c4a4d84d72e6900b06838210a76a8b.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>93300005349</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>364095686</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>36526</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="2" t="s">
+      <c r="H36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K36" s="3" t="str">
+      <c r="K36" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658662217643_ed95c6620651e7d00cbf14056e8b76fb.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L36" s="3" t="str">
+      <c r="L36" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658662210545_e4ce0c32a1d467887e7833d12cb4a286.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>89099008678</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="1">
+        <v>352503509</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="6" t="s">
+      <c r="D37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G37" s="7">
-        <v>44688</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="6" t="s">
+      <c r="G37" s="3">
+        <v>44747</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="6" t="s">
+      <c r="J37" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="K37" s="8" t="str">
+      <c r="K37" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658663234407_49b889c545ea800460ccfc5bd004abfc.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L37" s="8" t="str">
+      <c r="L37" s="2" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658663793134_2c4e81af8d38d8105d9c2186365b1a58.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>89088019851</v>
+      </c>
+      <c r="B38" s="5">
+        <v>351891756</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K38" s="6" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659032293123_4c7237225cac03719974481bc8dc0ab5.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L38" s="6" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659032298176_7a29562474990911c642bf7734211a7f.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>91081017072</v>
+      </c>
+      <c r="B39" s="11">
+        <v>370841245</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="12">
+        <v>29587</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="K39" s="13" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L39" s="13" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>92205005260</v>
+      </c>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="K40" s="15" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659098829266_d6ca5a653cecaa34d5e450ae9f10d090.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L40" s="15" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659098735032_dd8afed50c6c71bb10b6183cd5c28e8f.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="C1:C38" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Lê Hồng Phong"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
sao luu du lieu ngay 01/06/2025
</commit_message>
<xml_diff>
--- a/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
+++ b/APP_KHAI_BAO_LUU_TRU/DU_LIEU_KHAI_BAO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15909A5-4D21-4CCF-B7A4-C53C4AEE2DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF055AD-57A4-48EB-A2C0-A0B35A485C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB3A4D1C-0848-4C13-8670-93B20E72328E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="204">
   <si>
     <t>Số giấy tờ</t>
   </si>
@@ -579,6 +579,78 @@
   </si>
   <si>
     <t>21:55:02 31/05/2025</t>
+  </si>
+  <si>
+    <t>Trần Thị Linh</t>
+  </si>
+  <si>
+    <t>20/06/1991</t>
+  </si>
+  <si>
+    <t>Ấp 3, Phước Tuy, Cần Đước, Long An</t>
+  </si>
+  <si>
+    <t>23:28:55 31/05/2025</t>
+  </si>
+  <si>
+    <t>Trịnh Mỹ Linh</t>
+  </si>
+  <si>
+    <t>28/06/1981</t>
+  </si>
+  <si>
+    <t>Số Nhà 208/26/4/3 Đường Số 5, P.Bình Hưng Hòa, Bình Tân, TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>M145J8259</t>
+  </si>
+  <si>
+    <t>NA HANSUNG</t>
+  </si>
+  <si>
+    <t>14/03/2025</t>
+  </si>
+  <si>
+    <t>Hộ chiếu (passport)</t>
+  </si>
+  <si>
+    <t>M214P6196</t>
+  </si>
+  <si>
+    <t>DA SEONMI</t>
+  </si>
+  <si>
+    <t>27/07/1980</t>
+  </si>
+  <si>
+    <t>27/03/2025</t>
+  </si>
+  <si>
+    <t>M638G2538</t>
+  </si>
+  <si>
+    <t>BYUN YOUNGSOON</t>
+  </si>
+  <si>
+    <t>28/03/2025</t>
+  </si>
+  <si>
+    <t>M895N2213</t>
+  </si>
+  <si>
+    <t>RA CHUNHO</t>
+  </si>
+  <si>
+    <t>25/08/1953</t>
+  </si>
+  <si>
+    <t>Bành Văn Thuận</t>
+  </si>
+  <si>
+    <t>Ấp 6, Xà Phiên, Long Mỹ, Hậu Giang</t>
+  </si>
+  <si>
+    <t>Phòng 4 nhà cũ</t>
   </si>
 </sst>
 </file>
@@ -636,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -670,19 +742,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -698,22 +757,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,18 +766,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,31 +777,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1084,11 +1113,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:L40"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1129,7 @@
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="85.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -1108,1553 +1137,1789 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>91095006338</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="2">
         <v>371727089</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="8" t="str">
+      <c r="K2" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_Le_Quoc_Hiep_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L2" s="8" t="str">
+      <c r="L2" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_sau_Le_Quoc_Hiep_19_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>96193007157</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>33970</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="2" t="str">
+      <c r="K3" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_NGUYEN_THI_BICH_VAN_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L3" s="2" t="str">
+      <c r="L3" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_sau_NGUYEN_THI_BICH_VAN_19_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>56194006799</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="2" t="str">
+      <c r="K4" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\dist\Anh_CCCD_da_khai_bao\mat_truoc_TRAN_TIN_19_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>82079009889</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>25726188</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="2" t="str">
+      <c r="K5" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Huy_Binh_20_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L5" s="2" t="str">
+      <c r="L5" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Huy_Binh_20_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>75202005210</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="2" t="str">
+      <c r="K6" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_PHAN_HOANG_HIEU_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>51084019055</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>212772204</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4">
         <v>30682</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="2" t="str">
+      <c r="K7" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Duc_Danh_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L7" s="2" t="str">
+      <c r="L7" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Duc_Danh_21_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>91301013069</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>372037622</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="2" t="str">
+      <c r="K8" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Phuong_Thanh_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>89206019981</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4">
         <v>38751</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="2" t="str">
+      <c r="K9" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_PHAM_THANH_DONG_21_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>79095002950</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>25463058</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="2" t="str">
+      <c r="K10" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Tran_Phuc_Hau_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L10" s="2" t="str">
+      <c r="L10" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Tran_Phuc_Hau_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>91078008986</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>352465981</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="2" t="str">
+      <c r="K11" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Ngoc_Hong_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L11" s="2" t="str">
+      <c r="L11" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Ngoc_Hong_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>91097015554</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>371901334</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4">
         <v>35709</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="2" t="str">
+      <c r="K12" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_The_Hai_22_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L12" s="2" t="str">
+      <c r="L12" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_The_Hai_22_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>91071015623</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>371307162</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="2" t="str">
+      <c r="K13" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Nguyen_Thanh_Tuan_23_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L13" s="2" t="str">
+      <c r="L13" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Nguyen_Thanh_Tuan_23_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>87096015542</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K14" s="2" t="str">
+      <c r="K14" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_NGUYEN_MINH_TIEN_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L14" s="2" t="str">
+      <c r="L14" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_NGUYEN_MINH_TIEN_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="2">
         <v>91081017072</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="2">
         <v>370841245</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4">
         <v>29587</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="11" t="s">
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K15" s="13" t="str">
+      <c r="K15" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L15" s="13" t="str">
+      <c r="L15" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>91084012750</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="2">
         <v>370990818</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4">
         <v>30750</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="7" t="s">
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K16" s="8" t="str">
+      <c r="K16" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Thanh_Viet_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L16" s="8" t="str">
+      <c r="L16" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Thanh_Viet_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>1080001692</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>11897042</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="4">
         <v>45111</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K17" s="2" t="str">
+      <c r="K17" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Bui_Xuan_Khang_25_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>93089002224</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>363625191</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="K18" s="2" t="str">
+      <c r="K18" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231015986_1f8b3e3bff5db9556942e37df55eced1.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L18" s="2" t="str">
+      <c r="L18" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231009013_d0555d63762caa707a528779cd4b389d.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>92202000529</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="4">
         <v>37349</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="4">
         <v>44412</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="H19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K19" s="2" t="str">
+      <c r="K19" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638567942044_da6c7396bdb2fd41771af011ea2145c5.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L19" s="2" t="str">
+      <c r="L19" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638568010435_4cb996aca8b62ce8c532ac2c778dde52.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>91086020674</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>371101463</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="4">
         <v>31417</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="H20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K20" s="4" t="str">
+      <c r="K20" s="5" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Phan_Ngoc_Dang_26_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L20" s="4" t="str">
+      <c r="L20" s="5" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Phan_Ngoc_Dang_26_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>1073013937</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>23081798</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="H21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K21" s="2" t="str">
+      <c r="K21" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641706780560_8de2b94abdddf01864418a9ee361f149.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L21" s="2" t="str">
+      <c r="L21" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641706753500_4969ef17448d95fa7b72914b4214e313.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>89191014033</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>352357017</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="H22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K22" s="2" t="str">
+      <c r="K22" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641780724942_fb1294927028398d7950862fa21f9636.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L22" s="2" t="str">
+      <c r="L22" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641780715963_324045fc09999ad0544e5e88e11e507e.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>89195008544</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="H23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K23" s="2" t="str">
+      <c r="K23" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641990529491_dc032a7b7fed2b70e37151d2a537d76a.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L23" s="2" t="str">
+      <c r="L23" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6641990535137_0ba3595f83c73ecf5e97519d7e4f843a.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>91308000131</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="H24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K24" s="2" t="str">
+      <c r="K24" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6644316579444_f67de388d3d57ed3ae9a5e8306dccebb.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L24" s="2" t="str">
+      <c r="L24" s="3" t="str">
         <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6644316567657_6d508f7fbad3b912ebad7c3a2bde4ede.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>91090022191</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="1" t="s">
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="K25" s="2" t="str">
+      <c r="K25" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645679784460_16e9831700eec884b4672019a8e5bfd8.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L25" s="2" t="str">
+      <c r="L25" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645679849486_f2d97fe44df1a882fee4c3e556b460d2.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>87205017175</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>372056275</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="4">
         <v>45452</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="1" t="s">
+      <c r="H26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K26" s="2" t="str">
+      <c r="K26" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718598837_bba874eeeaee72f671be148520fa04b0.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L26" s="2" t="str">
+      <c r="L26" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718650512_7337cb5b825ec0567cc8354ba1923a63.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>86093011875</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>331682224</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="D27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="4">
         <v>44477</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="H27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K27" s="2" t="str">
+      <c r="K27" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718626247_43b23736a79c792015edd2e82b865f50.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L27" s="2" t="str">
+      <c r="L27" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6645718611344_84cf2a06806039ffa53b154dec78a339.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>91301013069</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>372037622</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="H28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K28" s="2" t="str">
+      <c r="K28" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6648835576244_a2b952b7970c5b96f3efe8aec6c5c6fe.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>91086004502</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="D29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="4">
         <v>31503</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="4">
         <v>45055</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="1" t="s">
+      <c r="H29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="K29" s="2" t="str">
+      <c r="K29" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6649363260209_12712fa4552842f9089d02cedb55b602.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L29" s="2" t="str">
+      <c r="L29" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6649363228340_9751bb18278ccc22aacbd35eeb4c3ab9.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>38203017024</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="1" t="s">
+      <c r="H30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="K30" s="2" t="str">
+      <c r="K30" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078531533_66d3cde5f7ba221f3215adeb3f6e8484.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L30" s="2" t="str">
+      <c r="L30" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078408443_5b3a0f504d4db5db6ac51ae06d0115b1.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>79089035969</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>24228060</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="D31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="H31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J31" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="K31" s="2" t="str">
+      <c r="K31" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6652066448631_e17daed702f5eb47520dac0a1edf6c01.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L31" s="2" t="str">
+      <c r="L31" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6652066391227_9ea3764b58b18c3479c831a588aef359.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>38203017024</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="1" t="s">
+      <c r="H32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="J32" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K32" s="2" t="str">
+      <c r="K32" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078531533_66d3cde5f7ba221f3215adeb3f6e8484.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L32" s="2" t="str">
+      <c r="L32" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6650078408443_5b3a0f504d4db5db6ac51ae06d0115b1.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>91086020674</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>371101463</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="4">
         <v>31417</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="1" t="s">
+      <c r="H33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J33" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>93089002224</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>363625191</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="1" t="s">
+      <c r="H34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="J34" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K34" s="2" t="str">
+      <c r="K34" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231015986_1f8b3e3bff5db9556942e37df55eced1.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L34" s="2" t="str">
+      <c r="L34" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6638231009013_d0555d63762caa707a528779cd4b389d.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>52095016049</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="D35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="4">
         <v>34792</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="1" t="s">
+      <c r="H35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J35" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="K35" s="2" t="str">
+      <c r="K35" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6655770392067_dac28a538906af34430c537091b09146.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L35" s="2" t="str">
+      <c r="L35" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6655770441419_e8c4a4d84d72e6900b06838210a76a8b.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>93300005349</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>364095686</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="4">
         <v>36526</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="1" t="s">
+      <c r="H36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="K36" s="2" t="str">
+      <c r="K36" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658662217643_ed95c6620651e7d00cbf14056e8b76fb.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L36" s="2" t="str">
+      <c r="L36" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658662210545_e4ce0c32a1d467887e7833d12cb4a286.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>89099008678</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>352503509</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="D37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="4">
         <v>44747</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="H37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J37" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K37" s="2" t="str">
+      <c r="K37" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658663234407_49b889c545ea800460ccfc5bd004abfc.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L37" s="2" t="str">
+      <c r="L37" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6658663793134_2c4e81af8d38d8105d9c2186365b1a58.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>89088019851</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="2">
         <v>351891756</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="5" t="s">
+      <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="5" t="s">
+      <c r="H38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K38" s="6" t="str">
+      <c r="K38" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659032293123_4c7237225cac03719974481bc8dc0ab5.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L38" s="6" t="str">
+      <c r="L38" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659032298176_7a29562474990911c642bf7734211a7f.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="A39" s="2">
         <v>91081017072</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="2">
         <v>370841245</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="12">
+      <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="4">
         <v>29587</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="11" t="s">
+      <c r="H39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J39" s="11" t="s">
+      <c r="J39" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="K39" s="13" t="str">
+      <c r="K39" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_truoc_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L39" s="13" t="str">
+      <c r="L39" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\mat_sau_Le_Hong_Phong_24_05_2025.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+      <c r="A40" s="2">
         <v>92205005260</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="14" t="s">
+      <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H40" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="14" t="s">
+      <c r="H40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="K40" s="15" t="str">
+      <c r="K40" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659098829266_d6ca5a653cecaa34d5e450ae9f10d090.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L40" s="15" t="str">
+      <c r="L40" s="3" t="str">
         <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6659098735032_dd8afed50c6c71bb10b6183cd5c28e8f.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>84191010177</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>91181000392</v>
+      </c>
+      <c r="B42" s="2">
+        <v>370847325</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G42" s="4">
+        <v>44896</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J42" s="6">
+        <v>45663.501782407409</v>
+      </c>
+      <c r="K42" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6660330041981_8074e396856d314b7ca2dfb30fc02e4a.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L42" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6660330052415_cd7d9b540065e9d86f34d1d82fc17f67.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="4">
+        <v>31784</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" s="6">
+        <v>45663.752280092594</v>
+      </c>
+      <c r="K43" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6661225461171_ff9170910942afb00617936d8ced0374.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J44" s="6">
+        <v>45663.754861111112</v>
+      </c>
+      <c r="K44" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6661225474169_9a6c1238a3ff3a9e15f862f669333802.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="4">
+        <v>35037</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J45" s="6">
+        <v>45663.756099537037</v>
+      </c>
+      <c r="K45" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6661225469482_df13a55c54c83b589ffc4e83c833526f.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="4">
+        <v>45749</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J46" s="6">
+        <v>45663.757060185184</v>
+      </c>
+      <c r="K46" s="3" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6661225469550_0943b128e0d6e4c4d28c65a998c1a8cd.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>95078003474</v>
+      </c>
+      <c r="B47" s="7">
+        <v>363946051</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="8">
+        <v>28491</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G47" s="8">
+        <v>44687</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="J47" s="9">
+        <v>45663.893854166665</v>
+      </c>
+      <c r="K47" s="10" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6661845711359_81a289c8ade427775e8df9c160394d8b.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L47" s="10" t="str">
+        <f>HYPERLINK("D:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU\Anh_CCCD_da_khai_bao\z6661845650409_138f6d5dbc38836f0866949a5835bf21.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C38" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Lê Hồng Phong"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:C42" xr:uid="{14F59D22-0997-424E-90C7-F59553FEA18B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>